<commit_message>
update FCA spreadsheet, removed temp term from larv sens neurons
</commit_message>
<xml_diff>
--- a/cell_type_reports/_FCA_cell_type_lists.xlsx
+++ b/cell_type_reports/_FCA_cell_type_lists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cp390/git/drosophila-anatomy-developmental-ontology/cell_type_reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33204F09-9354-8C48-9941-7DF689B527F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D60F247-6645-3A43-BEC0-C770B6549582}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25040" windowHeight="22940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -686,12 +686,6 @@
     <t>FBbt_00048484</t>
   </si>
   <si>
-    <t>embryonic/larval muscle system; larval cuticle part; embryonic/larval epidermis</t>
-  </si>
-  <si>
-    <t>FBbt_00000462; FBbt_00048483; FBbt_00005398</t>
-  </si>
-  <si>
     <t>adult_muscle_system_cells.xlsx
 adult_sensory_neurons.xlsx
 adult_cuticle_parts.xlsx</t>
@@ -706,12 +700,6 @@
     <t>adult_cuticle_parts.xslx</t>
   </si>
   <si>
-    <t>embryonic-larval_muscle_system_cells.xlsx; embryonic-larval_cuticle_parts.xlsx; embryonic-larval_epidermis_parts.xlsx</t>
-  </si>
-  <si>
-    <t>"part of" some cuticle and "part of" some larva; also sensory neurons?</t>
-  </si>
-  <si>
     <t>"sensory neuron" that "part of" some "adult nervous system"; "part of" some cuticle and "part of" some adult; no epidermis terms for adult</t>
   </si>
   <si>
@@ -738,6 +726,18 @@
   </si>
   <si>
     <t>embryonic-larval_tracheal_system_cells.xlsx</t>
+  </si>
+  <si>
+    <t>embryonic/larval muscle system; larval cuticle part; embryonic/larval epidermis; embryonic/larval sensory neuron</t>
+  </si>
+  <si>
+    <t>FBbt_00000462; FBbt_00048483; FBbt_00005398; FBbt_00048485</t>
+  </si>
+  <si>
+    <t>"part of" some cuticle and "part of" some larva; "sensory neuron" that "part of" some "embryonic/larval nervous system"</t>
+  </si>
+  <si>
+    <t>embryonic-larval_muscle_system_cells.xlsx; embryonic-larval_cuticle_parts.xlsx; embryonic-larval_epidermis_parts.xlsx; embryonic-larval_sensory_neurons.xlsx</t>
   </si>
 </sst>
 </file>
@@ -774,18 +774,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -800,14 +794,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1552,7 +1543,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39:E40"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1585,11 +1576,11 @@
       <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
@@ -1604,11 +1595,11 @@
       <c r="D2" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
@@ -1623,23 +1614,23 @@
       <c r="D3" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" ht="56" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>224</v>
+        <v>231</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="28" x14ac:dyDescent="0.15">
@@ -1647,7 +1638,7 @@
         <v>91</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>214</v>
@@ -1660,10 +1651,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="28" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>205</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1672,13 +1663,13 @@
       <c r="D6" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="28" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>210</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1687,7 +1678,7 @@
       <c r="D7" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
@@ -1702,8 +1693,8 @@
       <c r="D8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>227</v>
+      <c r="E8" s="5" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14" x14ac:dyDescent="0.15">
@@ -1719,7 +1710,7 @@
       <c r="D9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
@@ -1788,18 +1779,18 @@
         <v>103</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
@@ -1833,8 +1824,8 @@
       <c r="A17" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>226</v>
+      <c r="B17" s="5" t="s">
+        <v>222</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>8</v>
@@ -1842,11 +1833,11 @@
       <c r="D17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
@@ -1861,11 +1852,11 @@
       <c r="D18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
@@ -1880,7 +1871,7 @@
       <c r="D19" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
@@ -2183,30 +2174,30 @@
         <v>133</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="E39" s="6"/>
+        <v>224</v>
+      </c>
+      <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="E40" s="6"/>
+        <v>225</v>
+      </c>
+      <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">

</xml_diff>